<commit_message>
Ajout traductions et correction de code
</commit_message>
<xml_diff>
--- a/tools/skills translate.xlsx
+++ b/tools/skills translate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33619\Documents\GitHub\Trinity-Admin\TrinityAdmin\tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Trinity-Admin\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D90542-DC0A-45B9-8F9A-66779B807AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649B093D-C11D-432D-8A88-6AFFDEC0D796}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{183AB95E-60C3-4E64-BB22-BBF372FE1855}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$2:$K$250</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -6955,11 +6955,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F8331B-0190-47B4-AA03-F9BBE88A2224}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A2:R250"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A242" sqref="A242"/>
+      <selection activeCell="R3" sqref="R3:R250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7001,7 +7000,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="3" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>333</v>
       </c>
@@ -7040,11 +7039,11 @@
         <v>{ entry = 333, name = "Enchanting" },</v>
       </c>
       <c r="R3" t="str">
-        <f>"L["""&amp;D3&amp;"""] = """ &amp; B3 &amp; """"</f>
-        <v>L["Enchanting"] = "Enchantement"</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <f>"L["""&amp;D3&amp;"""] = """ &amp; K3 &amp; """"</f>
+        <v>L["Enchanting"] = "附魔"</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>202</v>
       </c>
@@ -7083,11 +7082,11 @@
         <v>{ entry = 202, name = "Engineering" },</v>
       </c>
       <c r="R4" t="str">
-        <f t="shared" ref="R4:R67" si="1">"L["""&amp;D4&amp;"""] = """ &amp; B4 &amp; """"</f>
-        <v>L["Engineering"] = "Ingénierie"</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" ref="R4:R67" si="1">"L["""&amp;D4&amp;"""] = """ &amp; K4 &amp; """"</f>
+        <v>L["Engineering"] = "工程学"</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>164</v>
       </c>
@@ -7127,10 +7126,10 @@
       </c>
       <c r="R5" t="str">
         <f t="shared" si="1"/>
-        <v>L["Blacksmithing"] = "Forge"</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Blacksmithing"] = "锻造"</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>773</v>
       </c>
@@ -7170,10 +7169,10 @@
       </c>
       <c r="R6" t="str">
         <f t="shared" si="1"/>
-        <v>L["Inscription"] = "Calligraphie"</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Inscription"] = "铭文"</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>197</v>
       </c>
@@ -7213,10 +7212,10 @@
       </c>
       <c r="R7" t="str">
         <f t="shared" si="1"/>
-        <v>L["Tailoring"] = "Couture"</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Tailoring"] = "裁缝"</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>755</v>
       </c>
@@ -7256,10 +7255,10 @@
       </c>
       <c r="R8" t="str">
         <f t="shared" si="1"/>
-        <v>L["Jewelcrafting"] = "Joaillerie"</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Jewelcrafting"] = "珠宝加工"</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>165</v>
       </c>
@@ -7299,10 +7298,10 @@
       </c>
       <c r="R9" t="str">
         <f t="shared" si="1"/>
-        <v>L["Leatherworking"] = "Travail du cuir"</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Leatherworking"] = "制皮"</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>171</v>
       </c>
@@ -7342,10 +7341,10 @@
       </c>
       <c r="R10" t="str">
         <f t="shared" si="1"/>
-        <v>L["Alchemy"] = "Alchimie"</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Alchemy"] = "炼金术"</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>794</v>
       </c>
@@ -7385,10 +7384,10 @@
       </c>
       <c r="R11" t="str">
         <f t="shared" si="1"/>
-        <v>L["Archaeology"] = "Archéologie"</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Archaeology"] = "考古学"</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>182</v>
       </c>
@@ -7428,10 +7427,10 @@
       </c>
       <c r="R12" t="str">
         <f t="shared" si="1"/>
-        <v>L["Herbalism"] = "Herboristerie"</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Herbalism"] = "草药学"</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>356</v>
       </c>
@@ -7471,10 +7470,10 @@
       </c>
       <c r="R13" t="str">
         <f t="shared" si="1"/>
-        <v>L["Fishing"] = "Pêche"</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Fishing"] = "钓鱼"</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>185</v>
       </c>
@@ -7514,10 +7513,10 @@
       </c>
       <c r="R14" t="str">
         <f t="shared" si="1"/>
-        <v>L["Cooking"] = "Cuisine"</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Cooking"] = "烹饪"</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>186</v>
       </c>
@@ -7557,10 +7556,10 @@
       </c>
       <c r="R15" t="str">
         <f t="shared" si="1"/>
-        <v>L["Mining"] = "Minage"</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Mining"] = "采矿"</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>762</v>
       </c>
@@ -7600,10 +7599,10 @@
       </c>
       <c r="R16" t="str">
         <f t="shared" si="1"/>
-        <v>L["Riding"] = "Monte"</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Riding"] = "骑术"</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>960</v>
       </c>
@@ -7643,10 +7642,10 @@
       </c>
       <c r="R17" t="str">
         <f t="shared" si="1"/>
-        <v>L["Runeforging"] = "Runeforge"</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Runeforging"] = "符文熔铸"</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>393</v>
       </c>
@@ -7686,10 +7685,10 @@
       </c>
       <c r="R18" t="str">
         <f t="shared" si="1"/>
-        <v>L["Skinning"] = "Dépeçage"</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Skinning"] = "剥皮"</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2875</v>
       </c>
@@ -7729,10 +7728,10 @@
       </c>
       <c r="R19" t="str">
         <f t="shared" si="1"/>
-        <v>L["Khaz Algar Engineering"] = "Ingénierie de Khaz Algar"</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Khaz Algar Engineering"] = "卡兹阿加工程学"</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2874</v>
       </c>
@@ -7772,10 +7771,10 @@
       </c>
       <c r="R20" t="str">
         <f t="shared" si="1"/>
-        <v>L["Khaz Algar Enchanting"] = "Enchantement de Khaz Algar"</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Khaz Algar Enchanting"] = "卡兹阿加附魔"</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>777</v>
       </c>
@@ -7815,10 +7814,10 @@
       </c>
       <c r="R21" t="str">
         <f t="shared" si="1"/>
-        <v>L["Mounts"] = "Montures"</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Mounts"] = "坐骑"</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2871</v>
       </c>
@@ -7858,10 +7857,10 @@
       </c>
       <c r="R22" t="str">
         <f t="shared" si="1"/>
-        <v>L["Khaz Algar Alchemy"] = "Alchimie de Khaz Algar"</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Khaz Algar Alchemy"] = "卡兹阿加炼金"</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2883</v>
       </c>
@@ -7901,10 +7900,10 @@
       </c>
       <c r="R23" t="str">
         <f t="shared" si="1"/>
-        <v>L["Khaz Algar Tailoring"] = "Couture de Khaz Algar"</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Khaz Algar Tailoring"] = "卡兹阿加裁缝"</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2528</v>
       </c>
@@ -7944,10 +7943,10 @@
       </c>
       <c r="R24" t="str">
         <f t="shared" si="1"/>
-        <v>L["Pandaria Leatherworking"] = "Travail du cuir de Pandarie"</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Pandaria Leatherworking"] = "潘达利亚制皮"</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2872</v>
       </c>
@@ -7987,10 +7986,10 @@
       </c>
       <c r="R25" t="str">
         <f t="shared" si="1"/>
-        <v>L["Khaz Algar Blacksmithing"] = "Forge de Khaz Algar"</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Khaz Algar Blacksmithing"] = "卡兹阿加锻造"</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2878</v>
       </c>
@@ -8030,10 +8029,10 @@
       </c>
       <c r="R26" t="str">
         <f t="shared" si="1"/>
-        <v>L["Khaz Algar Inscription"] = "Calligraphie de Khaz Algar"</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Khaz Algar Inscription"] = "卡兹阿加铭文"</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2881</v>
       </c>
@@ -8073,10 +8072,10 @@
       </c>
       <c r="R27" t="str">
         <f t="shared" si="1"/>
-        <v>L["Khaz Algar Mining"] = "Minage de Khaz Algar"</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Khaz Algar Mining"] = "卡兹阿加采矿"</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2880</v>
       </c>
@@ -8116,10 +8115,10 @@
       </c>
       <c r="R28" t="str">
         <f t="shared" si="1"/>
-        <v>L["Khaz Algar Leatherworking"] = "Travail du cuir de Khaz Algar"</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Khaz Algar Leatherworking"] = "卡兹阿加制皮"</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>160</v>
       </c>
@@ -8159,10 +8158,10 @@
       </c>
       <c r="R29" t="str">
         <f t="shared" si="1"/>
-        <v>L["Two-Handed Maces"] = "Masses à deux mains"</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Two-Handed Maces"] = "双手锤"</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2504</v>
       </c>
@@ -8202,10 +8201,10 @@
       </c>
       <c r="R30" t="str">
         <f t="shared" si="1"/>
-        <v>L["Northrend Engineering"] = "Ingénierie du Norfendre"</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Northrend Engineering"] = "诺森德工程学"</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>413</v>
       </c>
@@ -8245,10 +8244,10 @@
       </c>
       <c r="R31" t="str">
         <f t="shared" si="1"/>
-        <v>L["Mail"] = "Mailles"</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Mail"] = "锁甲"</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2879</v>
       </c>
@@ -8288,10 +8287,10 @@
       </c>
       <c r="R32" t="str">
         <f t="shared" si="1"/>
-        <v>L["Khaz Algar Jewelcrafting"] = "Joaillerie de Khaz Algar"</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Khaz Algar Jewelcrafting"] = "卡兹阿加珠宝加工"</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2873</v>
       </c>
@@ -8331,10 +8330,10 @@
       </c>
       <c r="R33" t="str">
         <f t="shared" si="1"/>
-        <v>L["Khaz Algar Cooking"] = "Cuisine de Khaz Algar"</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Khaz Algar Cooking"] = "卡兹阿加烹饪"</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2552</v>
       </c>
@@ -8374,10 +8373,10 @@
       </c>
       <c r="R34" t="str">
         <f t="shared" si="1"/>
-        <v>L["Pandaria Herbalism"] = "Herboristerie de Pandarie"</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Pandaria Herbalism"] = "潘达利亚草药学"</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2720</v>
       </c>
@@ -8417,10 +8416,10 @@
       </c>
       <c r="R35" t="str">
         <f t="shared" si="1"/>
-        <v>L["Junkyard Tinkering"] = "Bricolage de la casse"</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Junkyard Tinkering"] = "垃圾场匠技"</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2485</v>
       </c>
@@ -8460,10 +8459,10 @@
       </c>
       <c r="R36" t="str">
         <f t="shared" si="1"/>
-        <v>L["Classic Alchemy"] = "Alchimie classique"</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Classic Alchemy"] = "经典旧世炼金"</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2506</v>
       </c>
@@ -8503,10 +8502,10 @@
       </c>
       <c r="R37" t="str">
         <f t="shared" si="1"/>
-        <v>L["Classic Engineering"] = "Ingénierie classique"</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Classic Engineering"] = "经典旧世工程学"</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2882</v>
       </c>
@@ -8546,10 +8545,10 @@
       </c>
       <c r="R38" t="str">
         <f t="shared" si="1"/>
-        <v>L["Khaz Algar Skinning"] = "Dépeçage de Khaz Algar"</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Khaz Algar Skinning"] = "卡兹阿加剥皮"</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2734</v>
       </c>
@@ -8589,10 +8588,10 @@
       </c>
       <c r="R39" t="str">
         <f t="shared" si="1"/>
-        <v>L["Mount Equipment"] = "Équipement de monte"</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Mount Equipment"] = "坐骑装备"</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2876</v>
       </c>
@@ -8632,10 +8631,10 @@
       </c>
       <c r="R40" t="str">
         <f t="shared" si="1"/>
-        <v>L["Khaz Algar Fishing"] = "Pêche de Khaz Algar"</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Khaz Algar Fishing"] = "卡兹阿加钓鱼"</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2877</v>
       </c>
@@ -8675,10 +8674,10 @@
       </c>
       <c r="R41" t="str">
         <f t="shared" si="1"/>
-        <v>L["Khaz Algar Herbalism"] = "Herboristerie de Khaz Algar"</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Khaz Algar Herbalism"] = "卡兹阿加草药学"</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>54</v>
       </c>
@@ -8718,10 +8717,10 @@
       </c>
       <c r="R42" t="str">
         <f t="shared" si="1"/>
-        <v>L["Maces"] = "Masse"</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Maces"] = "单手锤"</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2505</v>
       </c>
@@ -8761,10 +8760,10 @@
       </c>
       <c r="R43" t="str">
         <f t="shared" si="1"/>
-        <v>L["Outland Engineering"] = "Ingénierie d’Outreterre"</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Outland Engineering"] = "外域工程学"</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2568</v>
       </c>
@@ -8804,10 +8803,10 @@
       </c>
       <c r="R44" t="str">
         <f t="shared" si="1"/>
-        <v>L["Pandaria Mining"] = "Minage de Pandarie"</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Pandaria Mining"] = "潘达利亚采矿"</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2521</v>
       </c>
@@ -8847,10 +8846,10 @@
       </c>
       <c r="R45" t="str">
         <f t="shared" si="1"/>
-        <v>L["Cataclysm Jewelcrafting"] = "Joaillerie de Cataclysm"</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Cataclysm Jewelcrafting"] = "大地的裂变珠宝加工"</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>414</v>
       </c>
@@ -8890,10 +8889,10 @@
       </c>
       <c r="R46" t="str">
         <f t="shared" si="1"/>
-        <v>L["Leather"] = "Cuir"</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Leather"] = "皮甲"</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>293</v>
       </c>
@@ -8933,10 +8932,10 @@
       </c>
       <c r="R47" t="str">
         <f t="shared" si="1"/>
-        <v>L["Plate Mail"] = "Armure en plaques"</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Plate Mail"] = "板甲"</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>904</v>
       </c>
@@ -8976,10 +8975,10 @@
       </c>
       <c r="R48" t="str">
         <f t="shared" si="1"/>
-        <v>L["Mage"] = "Mage"</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Mage"] = "法师"</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2727</v>
       </c>
@@ -9019,10 +9018,10 @@
       </c>
       <c r="R49" t="str">
         <f t="shared" si="1"/>
-        <v>L["All Classes"] = "Toutes les classes"</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["All Classes"] = "全职业"</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>46</v>
       </c>
@@ -9062,10 +9061,10 @@
       </c>
       <c r="R50" t="str">
         <f t="shared" si="1"/>
-        <v>L["Guns"] = "Armes à feu"</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Guns"] = "枪械"</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>229</v>
       </c>
@@ -9105,10 +9104,10 @@
       </c>
       <c r="R51" t="str">
         <f t="shared" si="1"/>
-        <v>L["Polearms"] = "Armes d'hast"</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Polearms"] = "长柄武器"</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2833</v>
       </c>
@@ -9148,10 +9147,10 @@
       </c>
       <c r="R52" t="str">
         <f t="shared" si="1"/>
-        <v>L["Dragon Isles Mining"] = "Minage des îles aux Dragons"</v>
-      </c>
-    </row>
-    <row r="53" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Dragon Isles Mining"] = "巨龙群岛采矿"</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2791</v>
       </c>
@@ -9191,10 +9190,10 @@
       </c>
       <c r="R53" t="str">
         <f t="shared" si="1"/>
-        <v>L["Ascension Crafting"] = "Artisanat de l’Ascension"</v>
-      </c>
-    </row>
-    <row r="54" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Ascension Crafting"] = "晋升工艺"</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2825</v>
       </c>
@@ -9234,10 +9233,10 @@
       </c>
       <c r="R54" t="str">
         <f t="shared" si="1"/>
-        <v>L["Dragon Isles Enchanting"] = "Enchantement des îles aux Dragons"</v>
-      </c>
-    </row>
-    <row r="55" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Dragon Isles Enchanting"] = "巨龙群岛附魔"</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>921</v>
       </c>
@@ -9277,10 +9276,10 @@
       </c>
       <c r="R55" t="str">
         <f t="shared" si="1"/>
-        <v>L["Rogue"] = "Voleur"</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Rogue"] = "潜行者"</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2499</v>
       </c>
@@ -9320,10 +9319,10 @@
       </c>
       <c r="R56" t="str">
         <f t="shared" si="1"/>
-        <v>L["Kul Tiran Engineering"] = "Ingénierie de Kul Tiras"</v>
-      </c>
-    </row>
-    <row r="57" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Kul Tiran Engineering"] = "库尔提拉斯工程学"</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>473</v>
       </c>
@@ -9363,10 +9362,10 @@
       </c>
       <c r="R57" t="str">
         <f t="shared" si="1"/>
-        <v>L["Fist Weapons"] = "Armes de pugilat"</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Fist Weapons"] = "拳套"</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2152</v>
       </c>
@@ -9406,10 +9405,10 @@
       </c>
       <c r="R58" t="str">
         <f t="shared" si="1"/>
-        <v>L["Warglaives"] = "Glaives de guerre"</v>
-      </c>
-    </row>
-    <row r="59" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Warglaives"] = "战刃"</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2566</v>
       </c>
@@ -9449,10 +9448,10 @@
       </c>
       <c r="R59" t="str">
         <f t="shared" si="1"/>
-        <v>L["Legion Mining"] = "Minage de Legion"</v>
-      </c>
-    </row>
-    <row r="60" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Legion Mining"] = "军团采矿"</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2902</v>
       </c>
@@ -9492,10 +9491,10 @@
       </c>
       <c r="R60" t="str">
         <f t="shared" si="1"/>
-        <v>L["All - Warbands"] = "Tout – Bataillons"</v>
-      </c>
-    </row>
-    <row r="61" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["All - Warbands"] = "全部 - 战团"</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>137</v>
       </c>
@@ -9535,10 +9534,10 @@
       </c>
       <c r="R61" t="str">
         <f t="shared" si="1"/>
-        <v>L["Thalassian"] = "thalassien"</v>
-      </c>
-    </row>
-    <row r="62" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Thalassian"] = "语言：萨拉斯语"</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>829</v>
       </c>
@@ -9578,10 +9577,10 @@
       </c>
       <c r="R62" t="str">
         <f t="shared" si="1"/>
-        <v>L["Monk"] = "Moine"</v>
-      </c>
-    </row>
-    <row r="63" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Monk"] = "武僧"</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2503</v>
       </c>
@@ -9621,10 +9620,10 @@
       </c>
       <c r="R63" t="str">
         <f t="shared" si="1"/>
-        <v>L["Cataclysm Engineering"] = "Ingénierie de Cataclysm"</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Cataclysm Engineering"] = "大地的裂变工程学"</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>98</v>
       </c>
@@ -9664,10 +9663,10 @@
       </c>
       <c r="R64" t="str">
         <f t="shared" si="1"/>
-        <v>L["Common"] = "commun"</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Common"] = "语言：通用语"</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>415</v>
       </c>
@@ -9707,10 +9706,10 @@
       </c>
       <c r="R65" t="str">
         <f t="shared" si="1"/>
-        <v>L["Cloth"] = "Tissu"</v>
-      </c>
-    </row>
-    <row r="66" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Cloth"] = "布甲"</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>924</v>
       </c>
@@ -9750,10 +9749,10 @@
       </c>
       <c r="R66" t="str">
         <f t="shared" si="1"/>
-        <v>L["Shaman"] = "Chaman"</v>
-      </c>
-    </row>
-    <row r="67" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Shaman"] = "萨满祭司"</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2540</v>
       </c>
@@ -9793,10 +9792,10 @@
       </c>
       <c r="R67" t="str">
         <f t="shared" si="1"/>
-        <v>L["Classic Tailoring"] = "Couture classique"</v>
-      </c>
-    </row>
-    <row r="68" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Classic Tailoring"] = "经典旧世裁缝"</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2542</v>
       </c>
@@ -9835,11 +9834,11 @@
         <v>{ entry = 2542, name = "Legion Cooking" },</v>
       </c>
       <c r="R68" t="str">
-        <f t="shared" ref="R68:R131" si="3">"L["""&amp;D68&amp;"""] = """ &amp; B68 &amp; """"</f>
-        <v>L["Legion Cooking"] = "Cuisine de Legion"</v>
-      </c>
-    </row>
-    <row r="69" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" ref="R68:R131" si="3">"L["""&amp;D68&amp;"""] = """ &amp; K68 &amp; """"</f>
+        <v>L["Legion Cooking"] = "军团烹饪"</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2567</v>
       </c>
@@ -9879,10 +9878,10 @@
       </c>
       <c r="R69" t="str">
         <f t="shared" si="3"/>
-        <v>L["Draenor Mining"] = "Minage de Draenor"</v>
-      </c>
-    </row>
-    <row r="70" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Draenor Mining"] = "德拉诺采矿"</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2730</v>
       </c>
@@ -9922,10 +9921,10 @@
       </c>
       <c r="R70" t="str">
         <f t="shared" si="3"/>
-        <v>L["Kyrian"] = "Kyrians"</v>
-      </c>
-    </row>
-    <row r="71" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Kyrian"] = "格里恩"</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2500</v>
       </c>
@@ -9965,10 +9964,10 @@
       </c>
       <c r="R71" t="str">
         <f t="shared" si="3"/>
-        <v>L["Legion Engineering"] = "Ingénierie de Legion"</v>
-      </c>
-    </row>
-    <row r="72" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Legion Engineering"] = "军团工程学"</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2553</v>
       </c>
@@ -10008,10 +10007,10 @@
       </c>
       <c r="R72" t="str">
         <f t="shared" si="3"/>
-        <v>L["Cataclysm Herbalism"] = "Herboristerie de Cataclysm"</v>
-      </c>
-    </row>
-    <row r="73" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Cataclysm Herbalism"] = "大地的裂变草药学"</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2831</v>
       </c>
@@ -10051,10 +10050,10 @@
       </c>
       <c r="R73" t="str">
         <f t="shared" si="3"/>
-        <v>L["Dragon Isles Tailoring"] = "Couture des îles aux Dragons"</v>
-      </c>
-    </row>
-    <row r="74" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Dragon Isles Tailoring"] = "巨龙群岛裁缝"</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2482</v>
       </c>
@@ -10094,10 +10093,10 @@
       </c>
       <c r="R74" t="str">
         <f t="shared" si="3"/>
-        <v>L["Cataclysm Alchemy"] = "Alchimie de Cataclysm"</v>
-      </c>
-    </row>
-    <row r="75" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Cataclysm Alchemy"] = "大地的裂变炼金"</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>172</v>
       </c>
@@ -10137,10 +10136,10 @@
       </c>
       <c r="R75" t="str">
         <f t="shared" si="3"/>
-        <v>L["Two-Handed Axes"] = "Haches à deux mains"</v>
-      </c>
-    </row>
-    <row r="76" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Two-Handed Axes"] = "双手斧"</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2477</v>
       </c>
@@ -10180,10 +10179,10 @@
       </c>
       <c r="R76" t="str">
         <f t="shared" si="3"/>
-        <v>L["Classic Blacksmithing"] = "Forge classique"</v>
-      </c>
-    </row>
-    <row r="77" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Classic Blacksmithing"] = "经典旧世锻造"</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2502</v>
       </c>
@@ -10223,10 +10222,10 @@
       </c>
       <c r="R77" t="str">
         <f t="shared" si="3"/>
-        <v>L["Pandaria Engineering"] = "Ingénierie de Pandarie"</v>
-      </c>
-    </row>
-    <row r="78" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Pandaria Engineering"] = "潘达利亚工程学"</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2520</v>
       </c>
@@ -10266,10 +10265,10 @@
       </c>
       <c r="R78" t="str">
         <f t="shared" si="3"/>
-        <v>L["Pandaria Jewelcrafting"] = "Joaillerie de Pandarie"</v>
-      </c>
-    </row>
-    <row r="79" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Pandaria Jewelcrafting"] = "潘达利亚珠宝加工"</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2756</v>
       </c>
@@ -10309,10 +10308,10 @@
       </c>
       <c r="R79" t="str">
         <f t="shared" si="3"/>
-        <v>L["Shadowlands Inscription"] = "Calligraphie d’Ombreterre"</v>
-      </c>
-    </row>
-    <row r="80" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Shadowlands Inscription"] = "暗影界铭文"</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2481</v>
       </c>
@@ -10352,10 +10351,10 @@
       </c>
       <c r="R80" t="str">
         <f t="shared" si="3"/>
-        <v>L["Pandaria Alchemy"] = "Alchimie de Pandarie"</v>
-      </c>
-    </row>
-    <row r="81" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Pandaria Alchemy"] = "潘达利亚炼金"</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>173</v>
       </c>
@@ -10395,7 +10394,7 @@
       </c>
       <c r="R81" t="str">
         <f t="shared" si="3"/>
-        <v>L["Daggers"] = "Dagues"</v>
+        <v>L["Daggers"] = "匕首"</v>
       </c>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.25">
@@ -10438,10 +10437,10 @@
       </c>
       <c r="R82" t="str">
         <f t="shared" si="3"/>
-        <v>L["Observer"] = "Observateur"</v>
-      </c>
-    </row>
-    <row r="83" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Observer"] = "眼魔"</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2544</v>
       </c>
@@ -10481,10 +10480,10 @@
       </c>
       <c r="R83" t="str">
         <f t="shared" si="3"/>
-        <v>L["Pandaria Cooking"] = "Cuisine de Pandarie"</v>
-      </c>
-    </row>
-    <row r="84" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Pandaria Cooking"] = "潘达利亚烹饪"</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2571</v>
       </c>
@@ -10524,10 +10523,10 @@
       </c>
       <c r="R84" t="str">
         <f t="shared" si="3"/>
-        <v>L["Outland Mining"] = "Minage d’Outreterre"</v>
-      </c>
-    </row>
-    <row r="85" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Outland Mining"] = "外域采矿"</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>43</v>
       </c>
@@ -10567,10 +10566,10 @@
       </c>
       <c r="R85" t="str">
         <f t="shared" si="3"/>
-        <v>L["Swords"] = "Epées"</v>
-      </c>
-    </row>
-    <row r="86" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Swords"] = "单手剑"</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2570</v>
       </c>
@@ -10610,10 +10609,10 @@
       </c>
       <c r="R86" t="str">
         <f t="shared" si="3"/>
-        <v>L["Northrend Mining"] = "Minage du Norfendre"</v>
-      </c>
-    </row>
-    <row r="87" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Northrend Mining"] = "诺森德采矿"</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2588</v>
       </c>
@@ -10653,10 +10652,10 @@
       </c>
       <c r="R87" t="str">
         <f t="shared" si="3"/>
-        <v>L["Pandaria Fishing"] = "Pêche de Pandarie"</v>
-      </c>
-    </row>
-    <row r="88" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Pandaria Fishing"] = "潘达利亚钓鱼"</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2829</v>
       </c>
@@ -10696,10 +10695,10 @@
       </c>
       <c r="R88" t="str">
         <f t="shared" si="3"/>
-        <v>L["Dragon Isles Jewelcrafting"] = "Joaillerie des îles aux Dragons"</v>
-      </c>
-    </row>
-    <row r="89" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Dragon Isles Jewelcrafting"] = "巨龙群岛珠宝加工"</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2847</v>
       </c>
@@ -10739,10 +10738,10 @@
       </c>
       <c r="R89" t="str">
         <f t="shared" si="3"/>
-        <v>L["Tuskarr Fishing Gear"] = "Matériel de pêche rohart"</v>
-      </c>
-    </row>
-    <row r="90" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Tuskarr Fishing Gear"] = "海象人渔具"</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>228</v>
       </c>
@@ -10782,10 +10781,10 @@
       </c>
       <c r="R90" t="str">
         <f t="shared" si="3"/>
-        <v>L["Wands"] = "Baguettes"</v>
-      </c>
-    </row>
-    <row r="91" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Wands"] = "魔杖"</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>1848</v>
       </c>
@@ -10825,10 +10824,10 @@
       </c>
       <c r="R91" t="str">
         <f t="shared" si="3"/>
-        <v>L["Demon Hunter"] = "Chasseur de démons"</v>
-      </c>
-    </row>
-    <row r="92" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Demon Hunter"] = "恶魔猎手"</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>2507</v>
       </c>
@@ -10868,10 +10867,10 @@
       </c>
       <c r="R92" t="str">
         <f t="shared" si="3"/>
-        <v>L["Kul Tiran Inscription"] = "Calligraphie de Kul Tiras"</v>
-      </c>
-    </row>
-    <row r="93" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Kul Tiran Inscription"] = "库尔提拉斯铭文"</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>2592</v>
       </c>
@@ -10911,10 +10910,10 @@
       </c>
       <c r="R93" t="str">
         <f t="shared" si="3"/>
-        <v>L["Classic Fishing"] = "Pêche classique"</v>
-      </c>
-    </row>
-    <row r="94" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Classic Fishing"] = "经典旧世钓鱼"</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>136</v>
       </c>
@@ -10954,10 +10953,10 @@
       </c>
       <c r="R94" t="str">
         <f t="shared" si="3"/>
-        <v>L["Staves"] = "Bâtons"</v>
-      </c>
-    </row>
-    <row r="95" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Staves"] = "法杖"</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>778</v>
       </c>
@@ -10997,10 +10996,10 @@
       </c>
       <c r="R95" t="str">
         <f t="shared" si="3"/>
-        <v>L["Companions"] = "Compagnons"</v>
-      </c>
-    </row>
-    <row r="96" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Companions"] = "小伙伴"</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>2493</v>
       </c>
@@ -11040,10 +11039,10 @@
       </c>
       <c r="R96" t="str">
         <f t="shared" si="3"/>
-        <v>L["Outland Enchanting"] = "Enchantement d’Outreterre"</v>
-      </c>
-    </row>
-    <row r="97" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Outland Enchanting"] = "外域附魔"</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2510</v>
       </c>
@@ -11083,10 +11082,10 @@
       </c>
       <c r="R97" t="str">
         <f t="shared" si="3"/>
-        <v>L["Pandaria Inscription"] = "Calligraphie de Pandarie"</v>
-      </c>
-    </row>
-    <row r="98" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Pandaria Inscription"] = "潘达利亚铭文"</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2546</v>
       </c>
@@ -11126,10 +11125,10 @@
       </c>
       <c r="R98" t="str">
         <f t="shared" si="3"/>
-        <v>L["Northrend Cooking"] = "Cuisine du Norfendre"</v>
-      </c>
-    </row>
-    <row r="99" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Northrend Cooking"] = "诺森德烹饪"</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2560</v>
       </c>
@@ -11169,10 +11168,10 @@
       </c>
       <c r="R99" t="str">
         <f t="shared" si="3"/>
-        <v>L["Pandaria Skinning"] = "Dépeçage de Pandarie"</v>
-      </c>
-    </row>
-    <row r="100" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Pandaria Skinning"] = "潘达利亚剥皮"</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2563</v>
       </c>
@@ -11212,10 +11211,10 @@
       </c>
       <c r="R100" t="str">
         <f t="shared" si="3"/>
-        <v>L["Outland Skinning"] = "Dépeçage d’Outreterre"</v>
-      </c>
-    </row>
-    <row r="101" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Outland Skinning"] = "外域剥皮"</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>2752</v>
       </c>
@@ -11255,10 +11254,10 @@
       </c>
       <c r="R101" t="str">
         <f t="shared" si="3"/>
-        <v>L["Shadowlands Cooking"] = "Cuisine d’Ombreterre"</v>
-      </c>
-    </row>
-    <row r="102" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Shadowlands Cooking"] = "暗影界烹饪"</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>2819</v>
       </c>
@@ -11298,10 +11297,10 @@
       </c>
       <c r="R102" t="str">
         <f t="shared" si="3"/>
-        <v>L["Protoform Synthesis"] = "Synthèse de protoforme"</v>
-      </c>
-    </row>
-    <row r="103" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Protoform Synthesis"] = "原生体合成"</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>1945</v>
       </c>
@@ -11341,10 +11340,10 @@
       </c>
       <c r="R103" t="str">
         <f t="shared" si="3"/>
-        <v>L["Logging"] = "Abattage"</v>
-      </c>
-    </row>
-    <row r="104" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Logging"] = "伐木"</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>2486</v>
       </c>
@@ -11384,10 +11383,10 @@
       </c>
       <c r="R104" t="str">
         <f t="shared" si="3"/>
-        <v>L["Kul Tiran Enchanting"] = "Enchantement de Kul Tiras"</v>
-      </c>
-    </row>
-    <row r="105" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Kul Tiran Enchanting"] = "库尔提拉斯附魔"</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>2533</v>
       </c>
@@ -11427,10 +11426,10 @@
       </c>
       <c r="R105" t="str">
         <f t="shared" si="3"/>
-        <v>L["Kul Tiran Tailoring"] = "Couture de Kul Tiras"</v>
-      </c>
-    </row>
-    <row r="106" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Kul Tiran Tailoring"] = "库尔提拉斯裁缝"</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>2564</v>
       </c>
@@ -11470,10 +11469,10 @@
       </c>
       <c r="R106" t="str">
         <f t="shared" si="3"/>
-        <v>L["Classic Skinning"] = "Dépeçage classique"</v>
-      </c>
-    </row>
-    <row r="107" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Classic Skinning"] = "经典旧世剥皮"</v>
+      </c>
+    </row>
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>45</v>
       </c>
@@ -11513,10 +11512,10 @@
       </c>
       <c r="R107" t="str">
         <f t="shared" si="3"/>
-        <v>L["Bows"] = "Arcs"</v>
-      </c>
-    </row>
-    <row r="108" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Bows"] = "弓"</v>
+      </c>
+    </row>
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>840</v>
       </c>
@@ -11556,10 +11555,10 @@
       </c>
       <c r="R108" t="str">
         <f t="shared" si="3"/>
-        <v>L["Warrior"] = "Guerrier"</v>
-      </c>
-    </row>
-    <row r="109" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Warrior"] = "战士"</v>
+      </c>
+    </row>
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>2538</v>
       </c>
@@ -11599,10 +11598,10 @@
       </c>
       <c r="R109" t="str">
         <f t="shared" si="3"/>
-        <v>L["Northrend Tailoring"] = "Couture du Norfendre"</v>
-      </c>
-    </row>
-    <row r="110" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Northrend Tailoring"] = "诺森德裁缝"</v>
+      </c>
+    </row>
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>2569</v>
       </c>
@@ -11642,10 +11641,10 @@
       </c>
       <c r="R110" t="str">
         <f t="shared" si="3"/>
-        <v>L["Cataclysm Mining"] = "Minage de Cataclysm"</v>
-      </c>
-    </row>
-    <row r="111" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Cataclysm Mining"] = "大地的裂变采矿"</v>
+      </c>
+    </row>
+    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>2787</v>
       </c>
@@ -11685,10 +11684,10 @@
       </c>
       <c r="R111" t="str">
         <f t="shared" si="3"/>
-        <v>L["Abominable Stitching"] = "Suture abominable"</v>
-      </c>
-    </row>
-    <row r="112" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Abominable Stitching"] = "憎恶缝合"</v>
+      </c>
+    </row>
+    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>2551</v>
       </c>
@@ -11728,10 +11727,10 @@
       </c>
       <c r="R112" t="str">
         <f t="shared" si="3"/>
-        <v>L["Draenor Herbalism"] = "Herboristerie de Draenor"</v>
-      </c>
-    </row>
-    <row r="113" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Draenor Herbalism"] = "德拉诺草药学"</v>
+      </c>
+    </row>
+    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>2830</v>
       </c>
@@ -11771,10 +11770,10 @@
       </c>
       <c r="R113" t="str">
         <f t="shared" si="3"/>
-        <v>L["Dragon Isles Leatherworking"] = "Travail du cuir des îles aux Dragons"</v>
-      </c>
-    </row>
-    <row r="114" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Dragon Isles Leatherworking"] = "巨龙群岛制皮"</v>
+      </c>
+    </row>
+    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>2846</v>
       </c>
@@ -11814,10 +11813,10 @@
       </c>
       <c r="R114" t="str">
         <f t="shared" si="3"/>
-        <v>L["Crafting"] = "Artisanat"</v>
-      </c>
-    </row>
-    <row r="115" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Crafting"] = "制造"</v>
+      </c>
+    </row>
+    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>55</v>
       </c>
@@ -11857,10 +11856,10 @@
       </c>
       <c r="R115" t="str">
         <f t="shared" si="3"/>
-        <v>L["Two-Handed Swords"] = "Epées à deux mains"</v>
-      </c>
-    </row>
-    <row r="116" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Two-Handed Swords"] = "双手剑"</v>
+      </c>
+    </row>
+    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>2480</v>
       </c>
@@ -11900,10 +11899,10 @@
       </c>
       <c r="R116" t="str">
         <f t="shared" si="3"/>
-        <v>L["Draenor Alchemy"] = "Alchimie de Draenor"</v>
-      </c>
-    </row>
-    <row r="117" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Draenor Alchemy"] = "德拉诺炼金"</v>
+      </c>
+    </row>
+    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>2513</v>
       </c>
@@ -11943,10 +11942,10 @@
       </c>
       <c r="R117" t="str">
         <f t="shared" si="3"/>
-        <v>L["Outland Inscription"] = "Calligraphie d’Outreterre"</v>
-      </c>
-    </row>
-    <row r="118" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Outland Inscription"] = "外域铭文"</v>
+      </c>
+    </row>
+    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>2562</v>
       </c>
@@ -11986,10 +11985,10 @@
       </c>
       <c r="R118" t="str">
         <f t="shared" si="3"/>
-        <v>L["Northrend Skinning"] = "Dépeçage du Norfendre"</v>
-      </c>
-    </row>
-    <row r="119" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Northrend Skinning"] = "诺森德剥皮"</v>
+      </c>
+    </row>
+    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>226</v>
       </c>
@@ -12029,10 +12028,10 @@
       </c>
       <c r="R119" t="str">
         <f t="shared" si="3"/>
-        <v>L["Crossbows"] = "Arbalètes"</v>
-      </c>
-    </row>
-    <row r="120" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Crossbows"] = "弩"</v>
+      </c>
+    </row>
+    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>315</v>
       </c>
@@ -12072,10 +12071,10 @@
       </c>
       <c r="R120" t="str">
         <f t="shared" si="3"/>
-        <v>L["Troll"] = "troll"</v>
-      </c>
-    </row>
-    <row r="121" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Troll"] = "语言：巨魔语"</v>
+      </c>
+    </row>
+    <row r="121" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>2478</v>
       </c>
@@ -12115,10 +12114,10 @@
       </c>
       <c r="R121" t="str">
         <f t="shared" si="3"/>
-        <v>L["Kul Tiran Alchemy"] = "Alchimie de Kul Tiras"</v>
-      </c>
-    </row>
-    <row r="122" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Kul Tiran Alchemy"] = "库尔提拉斯炼金术"</v>
+      </c>
+    </row>
+    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>2484</v>
       </c>
@@ -12158,10 +12157,10 @@
       </c>
       <c r="R122" t="str">
         <f t="shared" si="3"/>
-        <v>L["Outland Alchemy"] = "Alchimie d’Outreterre"</v>
-      </c>
-    </row>
-    <row r="123" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Outland Alchemy"] = "外域炼金"</v>
+      </c>
+    </row>
+    <row r="123" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>2536</v>
       </c>
@@ -12201,10 +12200,10 @@
       </c>
       <c r="R123" t="str">
         <f t="shared" si="3"/>
-        <v>L["Pandaria Tailoring"] = "Couture de Pandarie"</v>
-      </c>
-    </row>
-    <row r="124" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Pandaria Tailoring"] = "潘达利亚裁缝"</v>
+      </c>
+    </row>
+    <row r="124" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>2555</v>
       </c>
@@ -12244,10 +12243,10 @@
       </c>
       <c r="R124" t="str">
         <f t="shared" si="3"/>
-        <v>L["Outland Herbalism"] = "Herboristerie d’Outreterre"</v>
-      </c>
-    </row>
-    <row r="125" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Outland Herbalism"] = "外域草药学"</v>
+      </c>
+    </row>
+    <row r="125" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>2586</v>
       </c>
@@ -12287,10 +12286,10 @@
       </c>
       <c r="R125" t="str">
         <f t="shared" si="3"/>
-        <v>L["Legion Fishing"] = "Pêche de Legion"</v>
-      </c>
-    </row>
-    <row r="126" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Legion Fishing"] = "军团钓鱼"</v>
+      </c>
+    </row>
+    <row r="126" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>2760</v>
       </c>
@@ -12330,10 +12329,10 @@
       </c>
       <c r="R126" t="str">
         <f t="shared" si="3"/>
-        <v>L["Shadowlands Herbalism"] = "Herboristerie d’Ombreterre"</v>
-      </c>
-    </row>
-    <row r="127" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Shadowlands Herbalism"] = "暗影界草药学"</v>
+      </c>
+    </row>
+    <row r="127" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>2823</v>
       </c>
@@ -12373,10 +12372,10 @@
       </c>
       <c r="R127" t="str">
         <f t="shared" si="3"/>
-        <v>L["Dragon Isles Alchemy"] = "Alchimie des îles aux Dragons"</v>
-      </c>
-    </row>
-    <row r="128" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Dragon Isles Alchemy"] = "巨龙群岛炼金"</v>
+      </c>
+    </row>
+    <row r="128" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>2476</v>
       </c>
@@ -12416,10 +12415,10 @@
       </c>
       <c r="R128" t="str">
         <f t="shared" si="3"/>
-        <v>L["Outland Blacksmithing"] = "Forge d’Outreterre"</v>
-      </c>
-    </row>
-    <row r="129" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Outland Blacksmithing"] = "外域锻造"</v>
+      </c>
+    </row>
+    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>2731</v>
       </c>
@@ -12459,10 +12458,10 @@
       </c>
       <c r="R129" t="str">
         <f t="shared" si="3"/>
-        <v>L["Venthyr"] = "Venthyrs"</v>
-      </c>
-    </row>
-    <row r="130" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Venthyr"] = "温西尔"</v>
+      </c>
+    </row>
+    <row r="130" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>2834</v>
       </c>
@@ -12502,10 +12501,10 @@
       </c>
       <c r="R130" t="str">
         <f t="shared" si="3"/>
-        <v>L["Dragon Isles Skinning"] = "Dépeçage des îles aux Dragons"</v>
-      </c>
-    </row>
-    <row r="131" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Dragon Isles Skinning"] = "巨龙群岛剥皮"</v>
+      </c>
+    </row>
+    <row r="131" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>2479</v>
       </c>
@@ -12545,10 +12544,10 @@
       </c>
       <c r="R131" t="str">
         <f t="shared" si="3"/>
-        <v>L["Legion Alchemy"] = "Alchimie de Legion"</v>
-      </c>
-    </row>
-    <row r="132" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Legion Alchemy"] = "军团炼金"</v>
+      </c>
+    </row>
+    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>2488</v>
       </c>
@@ -12587,11 +12586,11 @@
         <v>{ entry = 2488, name = "Draenor Enchanting" },</v>
       </c>
       <c r="R132" t="str">
-        <f t="shared" ref="R132:R195" si="5">"L["""&amp;D132&amp;"""] = """ &amp; B132 &amp; """"</f>
-        <v>L["Draenor Enchanting"] = "Enchantement de Draenor"</v>
-      </c>
-    </row>
-    <row r="133" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" ref="R132:R195" si="5">"L["""&amp;D132&amp;"""] = """ &amp; K132 &amp; """"</f>
+        <v>L["Draenor Enchanting"] = "德拉诺附魔"</v>
+      </c>
+    </row>
+    <row r="133" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>2494</v>
       </c>
@@ -12631,10 +12630,10 @@
       </c>
       <c r="R133" t="str">
         <f t="shared" si="5"/>
-        <v>L["Classic Enchanting"] = "Enchantement classique"</v>
-      </c>
-    </row>
-    <row r="134" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Classic Enchanting"] = "经典旧世附魔"</v>
+      </c>
+    </row>
+    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>2545</v>
       </c>
@@ -12674,10 +12673,10 @@
       </c>
       <c r="R134" t="str">
         <f t="shared" si="5"/>
-        <v>L["Cataclysm Cooking"] = "Cuisine de Cataclysm"</v>
-      </c>
-    </row>
-    <row r="135" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Cataclysm Cooking"] = "大地的裂变烹饪"</v>
+      </c>
+    </row>
+    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>2816</v>
       </c>
@@ -12717,10 +12716,10 @@
       </c>
       <c r="R135" t="str">
         <f t="shared" si="5"/>
-        <v>L["Adventurer"] = "Aventurier ou aventurière"</v>
-      </c>
-    </row>
-    <row r="136" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Adventurer"] = "冒险者"</v>
+      </c>
+    </row>
+    <row r="136" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>2828</v>
       </c>
@@ -12760,10 +12759,10 @@
       </c>
       <c r="R136" t="str">
         <f t="shared" si="5"/>
-        <v>L["Dragon Isles Inscription"] = "Calligraphie des îles aux Dragons"</v>
-      </c>
-    </row>
-    <row r="137" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Dragon Isles Inscription"] = "巨龙群岛铭文"</v>
+      </c>
+    </row>
+    <row r="137" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>2437</v>
       </c>
@@ -12803,10 +12802,10 @@
       </c>
       <c r="R137" t="str">
         <f t="shared" si="5"/>
-        <v>L["Kul Tiran Blacksmithing"] = "Forge de Kul Tiras"</v>
-      </c>
-    </row>
-    <row r="138" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Kul Tiran Blacksmithing"] = "库尔提拉斯锻造"</v>
+      </c>
+    </row>
+    <row r="138" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>2475</v>
       </c>
@@ -12846,10 +12845,10 @@
       </c>
       <c r="R138" t="str">
         <f t="shared" si="5"/>
-        <v>L["Northrend Blacksmithing"] = "Forge du Norfendre"</v>
-      </c>
-    </row>
-    <row r="139" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Northrend Blacksmithing"] = "诺森德锻造"</v>
+      </c>
+    </row>
+    <row r="139" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>2501</v>
       </c>
@@ -12889,10 +12888,10 @@
       </c>
       <c r="R139" t="str">
         <f t="shared" si="5"/>
-        <v>L["Draenor Engineering"] = "Ingénierie de Draenor"</v>
-      </c>
-    </row>
-    <row r="140" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Draenor Engineering"] = "德拉诺工程学"</v>
+      </c>
+    </row>
+    <row r="140" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>2522</v>
       </c>
@@ -12932,10 +12931,10 @@
       </c>
       <c r="R140" t="str">
         <f t="shared" si="5"/>
-        <v>L["Northrend Jewelcrafting"] = "Joaillerie du Norfendre"</v>
-      </c>
-    </row>
-    <row r="141" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Northrend Jewelcrafting"] = "诺森德珠宝加工"</v>
+      </c>
+    </row>
+    <row r="141" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>2548</v>
       </c>
@@ -12975,10 +12974,10 @@
       </c>
       <c r="R141" t="str">
         <f t="shared" si="5"/>
-        <v>L["Classic Cooking"] = "Cuisine classique"</v>
-      </c>
-    </row>
-    <row r="142" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Classic Cooking"] = "经典旧世烹饪"</v>
+      </c>
+    </row>
+    <row r="142" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>2557</v>
       </c>
@@ -13018,10 +13017,10 @@
       </c>
       <c r="R142" t="str">
         <f t="shared" si="5"/>
-        <v>L["Kul Tiran Skinning"] = "Dépeçage de Kul Tiras"</v>
-      </c>
-    </row>
-    <row r="143" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Kul Tiran Skinning"] = "库尔提拉斯剥皮"</v>
+      </c>
+    </row>
+    <row r="143" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>2561</v>
       </c>
@@ -13061,10 +13060,10 @@
       </c>
       <c r="R143" t="str">
         <f t="shared" si="5"/>
-        <v>L["Cataclysm Skinning"] = "Dépeçage de Cataclysm"</v>
-      </c>
-    </row>
-    <row r="144" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Cataclysm Skinning"] = "大地的裂变剥皮"</v>
+      </c>
+    </row>
+    <row r="144" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>2585</v>
       </c>
@@ -13104,10 +13103,10 @@
       </c>
       <c r="R144" t="str">
         <f t="shared" si="5"/>
-        <v>L["Kul Tiran Fishing"] = "Pêche de Kul Tiras"</v>
-      </c>
-    </row>
-    <row r="145" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Kul Tiran Fishing"] = "库尔提拉斯钓鱼"</v>
+      </c>
+    </row>
+    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>2591</v>
       </c>
@@ -13147,7 +13146,7 @@
       </c>
       <c r="R145" t="str">
         <f t="shared" si="5"/>
-        <v>L["Outland Fishing"] = "Pêche d’Outreterre"</v>
+        <v>L["Outland Fishing"] = "外域钓鱼"</v>
       </c>
     </row>
     <row r="146" spans="1:18" x14ac:dyDescent="0.25">
@@ -13190,10 +13189,10 @@
       </c>
       <c r="R146" t="str">
         <f t="shared" si="5"/>
-        <v>L["Pet - Exotic Pterrordax"] = "Familier - pterreurdactyle exotique"</v>
-      </c>
-    </row>
-    <row r="147" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Pet - Exotic Pterrordax"] = "宠物 - 翼手龙（特殊）"</v>
+      </c>
+    </row>
+    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>2732</v>
       </c>
@@ -13233,10 +13232,10 @@
       </c>
       <c r="R147" t="str">
         <f t="shared" si="5"/>
-        <v>L["Night Fae"] = "Faë nocturnes"</v>
-      </c>
-    </row>
-    <row r="148" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Night Fae"] = "法夜"</v>
+      </c>
+    </row>
+    <row r="148" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>2733</v>
       </c>
@@ -13276,10 +13275,10 @@
       </c>
       <c r="R148" t="str">
         <f t="shared" si="5"/>
-        <v>L["Necrolord"] = "Nécro-seigneurs"</v>
-      </c>
-    </row>
-    <row r="149" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Necrolord"] = "通灵领主"</v>
+      </c>
+    </row>
+    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>2755</v>
       </c>
@@ -13319,10 +13318,10 @@
       </c>
       <c r="R149" t="str">
         <f t="shared" si="5"/>
-        <v>L["Shadowlands Engineering"] = "Ingénierie d’Ombreterre"</v>
-      </c>
-    </row>
-    <row r="150" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Shadowlands Engineering"] = "暗影界工程学"</v>
+      </c>
+    </row>
+    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>2757</v>
       </c>
@@ -13362,10 +13361,10 @@
       </c>
       <c r="R150" t="str">
         <f t="shared" si="5"/>
-        <v>L["Shadowlands Jewelcrafting"] = "Joaillerie d’Ombreterre"</v>
-      </c>
-    </row>
-    <row r="151" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Shadowlands Jewelcrafting"] = "暗影界珠宝加工"</v>
+      </c>
+    </row>
+    <row r="151" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>2810</v>
       </c>
@@ -13405,10 +13404,10 @@
       </c>
       <c r="R151" t="str">
         <f t="shared" si="5"/>
-        <v>L["Evoker"] = "Évocateur"</v>
-      </c>
-    </row>
-    <row r="152" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Evoker"] = "唤魔师"</v>
+      </c>
+    </row>
+    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>433</v>
       </c>
@@ -13448,10 +13447,10 @@
       </c>
       <c r="R152" t="str">
         <f t="shared" si="5"/>
-        <v>L["Shield"] = "Bouclier"</v>
-      </c>
-    </row>
-    <row r="153" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Shield"] = "盾牌"</v>
+      </c>
+    </row>
+    <row r="153" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>2454</v>
       </c>
@@ -13491,10 +13490,10 @@
       </c>
       <c r="R153" t="str">
         <f t="shared" si="5"/>
-        <v>L["Legion Blacksmithing"] = "Forge de Legion"</v>
-      </c>
-    </row>
-    <row r="154" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Legion Blacksmithing"] = "军团锻造"</v>
+      </c>
+    </row>
+    <row r="154" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>2537</v>
       </c>
@@ -13534,10 +13533,10 @@
       </c>
       <c r="R154" t="str">
         <f t="shared" si="5"/>
-        <v>L["Cataclysm Tailoring"] = "Couture de Cataclysm"</v>
-      </c>
-    </row>
-    <row r="155" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Cataclysm Tailoring"] = "大地的裂变裁缝"</v>
+      </c>
+    </row>
+    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>2822</v>
       </c>
@@ -13577,10 +13576,10 @@
       </c>
       <c r="R155" t="str">
         <f t="shared" si="5"/>
-        <v>L["Dragon Isles Blacksmithing"] = "Forge des îles aux Dragons"</v>
-      </c>
-    </row>
-    <row r="156" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Dragon Isles Blacksmithing"] = "巨龙群岛锻造"</v>
+      </c>
+    </row>
+    <row r="156" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>2832</v>
       </c>
@@ -13620,10 +13619,10 @@
       </c>
       <c r="R156" t="str">
         <f t="shared" si="5"/>
-        <v>L["Dragon Isles Herbalism"] = "Herboristerie des îles aux Dragons"</v>
-      </c>
-    </row>
-    <row r="157" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Dragon Isles Herbalism"] = "巨龙群岛草药学"</v>
+      </c>
+    </row>
+    <row r="157" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>313</v>
       </c>
@@ -13663,10 +13662,10 @@
       </c>
       <c r="R157" t="str">
         <f t="shared" si="5"/>
-        <v>L["Gnomish"] = "gnome"</v>
-      </c>
-    </row>
-    <row r="158" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Gnomish"] = "语言：侏儒语"</v>
+      </c>
+    </row>
+    <row r="158" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>2523</v>
       </c>
@@ -13706,10 +13705,10 @@
       </c>
       <c r="R158" t="str">
         <f t="shared" si="5"/>
-        <v>L["Outland Jewelcrafting"] = "Joaillerie d’Outreterre"</v>
-      </c>
-    </row>
-    <row r="159" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Outland Jewelcrafting"] = "外域珠宝加工"</v>
+      </c>
+    </row>
+    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>2532</v>
       </c>
@@ -13749,10 +13748,10 @@
       </c>
       <c r="R159" t="str">
         <f t="shared" si="5"/>
-        <v>L["Classic Leatherworking"] = "Travail du cuir classique"</v>
-      </c>
-    </row>
-    <row r="160" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Classic Leatherworking"] = "经典旧世制皮"</v>
+      </c>
+    </row>
+    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>2543</v>
       </c>
@@ -13792,10 +13791,10 @@
       </c>
       <c r="R160" t="str">
         <f t="shared" si="5"/>
-        <v>L["Draenor Cooking"] = "Cuisine de Draenor"</v>
-      </c>
-    </row>
-    <row r="161" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Draenor Cooking"] = "德拉诺烹饪"</v>
+      </c>
+    </row>
+    <row r="161" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>2549</v>
       </c>
@@ -13835,10 +13834,10 @@
       </c>
       <c r="R161" t="str">
         <f t="shared" si="5"/>
-        <v>L["Kul Tiran Herbalism"] = "Herboristerie de Kul Tiras"</v>
-      </c>
-    </row>
-    <row r="162" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Kul Tiran Herbalism"] = "库尔提拉斯草药学"</v>
+      </c>
+    </row>
+    <row r="162" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>2556</v>
       </c>
@@ -13878,10 +13877,10 @@
       </c>
       <c r="R162" t="str">
         <f t="shared" si="5"/>
-        <v>L["Classic Herbalism"] = "Herboristerie classique"</v>
-      </c>
-    </row>
-    <row r="163" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Classic Herbalism"] = "经典旧世草药学"</v>
+      </c>
+    </row>
+    <row r="163" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>2590</v>
       </c>
@@ -13921,10 +13920,10 @@
       </c>
       <c r="R163" t="str">
         <f t="shared" si="5"/>
-        <v>L["Northrend Fishing"] = "Pêche du Norfendre"</v>
-      </c>
-    </row>
-    <row r="164" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Northrend Fishing"] = "诺森德钓鱼"</v>
+      </c>
+    </row>
+    <row r="164" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>2776</v>
       </c>
@@ -13964,10 +13963,10 @@
       </c>
       <c r="R164" t="str">
         <f t="shared" si="5"/>
-        <v>L["Vulpera"] = "vulpérin"</v>
-      </c>
-    </row>
-    <row r="165" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Vulpera"] = "语言：狐人语"</v>
+      </c>
+    </row>
+    <row r="165" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>2821</v>
       </c>
@@ -14007,10 +14006,10 @@
       </c>
       <c r="R165" t="str">
         <f t="shared" si="5"/>
-        <v>L["Arcana Manipulation"] = "Manipulation des arcanes"</v>
-      </c>
-    </row>
-    <row r="166" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Arcana Manipulation"] = "奥能操控"</v>
+      </c>
+    </row>
+    <row r="166" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>2824</v>
       </c>
@@ -14050,10 +14049,10 @@
       </c>
       <c r="R166" t="str">
         <f t="shared" si="5"/>
-        <v>L["Dragon Isles Cooking"] = "Cuisine des îles aux Dragons"</v>
-      </c>
-    </row>
-    <row r="167" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Dragon Isles Cooking"] = "巨龙群岛烹饪"</v>
+      </c>
+    </row>
+    <row r="167" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>44</v>
       </c>
@@ -14093,10 +14092,10 @@
       </c>
       <c r="R167" t="str">
         <f t="shared" si="5"/>
-        <v>L["Axes"] = "Haches"</v>
-      </c>
-    </row>
-    <row r="168" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Axes"] = "单手斧"</v>
+      </c>
+    </row>
+    <row r="168" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>113</v>
       </c>
@@ -14136,10 +14135,10 @@
       </c>
       <c r="R168" t="str">
         <f t="shared" si="5"/>
-        <v>L["Darnassian"] = "darnassien"</v>
-      </c>
-    </row>
-    <row r="169" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Darnassian"] = "语言：达纳苏斯语"</v>
+      </c>
+    </row>
+    <row r="169" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>2527</v>
       </c>
@@ -14179,10 +14178,10 @@
       </c>
       <c r="R169" t="str">
         <f t="shared" si="5"/>
-        <v>L["Draenor Leatherworking"] = "Travail du cuir de Draenor"</v>
-      </c>
-    </row>
-    <row r="170" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Draenor Leatherworking"] = "德拉诺制皮"</v>
+      </c>
+    </row>
+    <row r="170" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>2539</v>
       </c>
@@ -14222,10 +14221,10 @@
       </c>
       <c r="R170" t="str">
         <f t="shared" si="5"/>
-        <v>L["Outland Tailoring"] = "Couture d’Outreterre"</v>
-      </c>
-    </row>
-    <row r="171" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Outland Tailoring"] = "外域裁缝"</v>
+      </c>
+    </row>
+    <row r="171" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>2547</v>
       </c>
@@ -14265,7 +14264,7 @@
       </c>
       <c r="R171" t="str">
         <f t="shared" si="5"/>
-        <v>L["Outland Cooking"] = "Cuisine d’Outreterre"</v>
+        <v>L["Outland Cooking"] = "外域烹饪"</v>
       </c>
     </row>
     <row r="172" spans="1:18" x14ac:dyDescent="0.25">
@@ -14308,10 +14307,10 @@
       </c>
       <c r="R172" t="str">
         <f t="shared" si="5"/>
-        <v>L["Pet - Mammoth"] = "Familier - mammouth"</v>
-      </c>
-    </row>
-    <row r="173" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Pet - Mammoth"] = "宠物 - 猛犸象"</v>
+      </c>
+    </row>
+    <row r="173" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>2472</v>
       </c>
@@ -14351,10 +14350,10 @@
       </c>
       <c r="R173" t="str">
         <f t="shared" si="5"/>
-        <v>L["Draenor Blacksmithing"] = "Forge de Draenor"</v>
-      </c>
-    </row>
-    <row r="174" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Draenor Blacksmithing"] = "德拉诺锻造"</v>
+      </c>
+    </row>
+    <row r="174" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>2491</v>
       </c>
@@ -14394,10 +14393,10 @@
       </c>
       <c r="R174" t="str">
         <f t="shared" si="5"/>
-        <v>L["Cataclysm Enchanting"] = "Enchantement de Cataclysm"</v>
-      </c>
-    </row>
-    <row r="175" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Cataclysm Enchanting"] = "大地的裂变附魔"</v>
+      </c>
+    </row>
+    <row r="175" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>2524</v>
       </c>
@@ -14437,10 +14436,10 @@
       </c>
       <c r="R175" t="str">
         <f t="shared" si="5"/>
-        <v>L["Classic Jewelcrafting"] = "Joaillerie classique"</v>
-      </c>
-    </row>
-    <row r="176" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Classic Jewelcrafting"] = "经典旧世珠宝加工"</v>
+      </c>
+    </row>
+    <row r="176" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>2525</v>
       </c>
@@ -14480,10 +14479,10 @@
       </c>
       <c r="R176" t="str">
         <f t="shared" si="5"/>
-        <v>L["Kul Tiran Leatherworking"] = "Travail du cuir de Kul Tiras"</v>
-      </c>
-    </row>
-    <row r="177" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Kul Tiran Leatherworking"] = "库尔提拉斯制皮"</v>
+      </c>
+    </row>
+    <row r="177" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>2554</v>
       </c>
@@ -14523,10 +14522,10 @@
       </c>
       <c r="R177" t="str">
         <f t="shared" si="5"/>
-        <v>L["Northrend Herbalism"] = "Herboristerie du Norfendre"</v>
-      </c>
-    </row>
-    <row r="178" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Northrend Herbalism"] = "诺森德草药学"</v>
+      </c>
+    </row>
+    <row r="178" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>2565</v>
       </c>
@@ -14566,10 +14565,10 @@
       </c>
       <c r="R178" t="str">
         <f t="shared" si="5"/>
-        <v>L["Kul Tiran Mining"] = "Minage de Kul Tiras"</v>
-      </c>
-    </row>
-    <row r="179" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Kul Tiran Mining"] = "库尔提拉斯采矿"</v>
+      </c>
+    </row>
+    <row r="179" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>2572</v>
       </c>
@@ -14609,10 +14608,10 @@
       </c>
       <c r="R179" t="str">
         <f t="shared" si="5"/>
-        <v>L["Classic Mining"] = "Minage classique"</v>
-      </c>
-    </row>
-    <row r="180" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Classic Mining"] = "经典旧世采矿"</v>
+      </c>
+    </row>
+    <row r="180" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>2704</v>
       </c>
@@ -14652,10 +14651,10 @@
       </c>
       <c r="R180" t="str">
         <f t="shared" si="5"/>
-        <v>L["Pet - Horse"] = "Familier - cheval"</v>
-      </c>
-    </row>
-    <row r="181" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Pet - Horse"] = "宠物 - 马"</v>
+      </c>
+    </row>
+    <row r="181" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>2754</v>
       </c>
@@ -14695,10 +14694,10 @@
       </c>
       <c r="R181" t="str">
         <f t="shared" si="5"/>
-        <v>L["Shadowlands Fishing"] = "Pêche d’Ombreterre"</v>
-      </c>
-    </row>
-    <row r="182" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Shadowlands Fishing"] = "暗影界钓鱼"</v>
+      </c>
+    </row>
+    <row r="182" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>2758</v>
       </c>
@@ -14738,10 +14737,10 @@
       </c>
       <c r="R182" t="str">
         <f t="shared" si="5"/>
-        <v>L["Shadowlands Leatherworking"] = "Travail du cuir d’Ombreterre"</v>
-      </c>
-    </row>
-    <row r="183" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Shadowlands Leatherworking"] = "暗影界制皮"</v>
+      </c>
+    </row>
+    <row r="183" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>2855</v>
       </c>
@@ -14781,10 +14780,10 @@
       </c>
       <c r="R183" t="str">
         <f t="shared" si="5"/>
-        <v>L["Furbolg"] = "furbolg"</v>
-      </c>
-    </row>
-    <row r="184" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Furbolg"] = "语言：熊怪语"</v>
+      </c>
+    </row>
+    <row r="184" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>2884</v>
       </c>
@@ -14824,10 +14823,10 @@
       </c>
       <c r="R184" t="str">
         <f t="shared" si="5"/>
-        <v>L["Earthen"] = "terrestre"</v>
-      </c>
-    </row>
-    <row r="185" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Earthen"] = "语言：土灵语"</v>
+      </c>
+    </row>
+    <row r="185" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>109</v>
       </c>
@@ -14867,10 +14866,10 @@
       </c>
       <c r="R185" t="str">
         <f t="shared" si="5"/>
-        <v>L["Orcish"] = "orc"</v>
-      </c>
-    </row>
-    <row r="186" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Orcish"] = "语言：兽人语"</v>
+      </c>
+    </row>
+    <row r="186" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>111</v>
       </c>
@@ -14910,10 +14909,10 @@
       </c>
       <c r="R186" t="str">
         <f t="shared" si="5"/>
-        <v>L["Dwarven"] = "nain"</v>
-      </c>
-    </row>
-    <row r="187" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Dwarven"] = "语言：矮人语"</v>
+      </c>
+    </row>
+    <row r="187" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>791</v>
       </c>
@@ -14953,10 +14952,10 @@
       </c>
       <c r="R187" t="str">
         <f t="shared" si="5"/>
-        <v>L["Gilnean"] = "gilnéen"</v>
-      </c>
-    </row>
-    <row r="188" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Gilnean"] = "语言：吉尔尼斯语"</v>
+      </c>
+    </row>
+    <row r="188" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>849</v>
       </c>
@@ -14996,10 +14995,10 @@
       </c>
       <c r="R188" t="str">
         <f t="shared" si="5"/>
-        <v>L["Warlock"] = "Démoniste"</v>
-      </c>
-    </row>
-    <row r="189" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Warlock"] = "术士"</v>
+      </c>
+    </row>
+    <row r="189" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>981</v>
       </c>
@@ -15039,7 +15038,7 @@
       </c>
       <c r="R189" t="str">
         <f t="shared" si="5"/>
-        <v>L["Apprentice Cooking"] = "Apprenti cuisinier"</v>
+        <v>L["Apprentice Cooking"] = "学徒烹饪"</v>
       </c>
     </row>
     <row r="190" spans="1:18" x14ac:dyDescent="0.25">
@@ -15082,7 +15081,7 @@
       </c>
       <c r="R190" t="str">
         <f t="shared" si="5"/>
-        <v>L["Pet - Mechanical"] = "Familier - machine"</v>
+        <v>L["Pet - Mechanical"] = "宠物 - 机械"</v>
       </c>
     </row>
     <row r="191" spans="1:18" x14ac:dyDescent="0.25">
@@ -15125,7 +15124,7 @@
       </c>
       <c r="R191" t="str">
         <f t="shared" si="5"/>
-        <v>L["Pet - Abomination"] = "Familier - abomination"</v>
+        <v>L["Pet - Abomination"] = "宠物 - 憎恶"</v>
       </c>
     </row>
     <row r="192" spans="1:18" x14ac:dyDescent="0.25">
@@ -15168,7 +15167,7 @@
       </c>
       <c r="R192" t="str">
         <f t="shared" si="5"/>
-        <v>L["Pet - Oxen"] = "Familier - bovin"</v>
+        <v>L["Pet - Oxen"] = "宠物 - 牛"</v>
       </c>
     </row>
     <row r="193" spans="1:18" x14ac:dyDescent="0.25">
@@ -15211,10 +15210,10 @@
       </c>
       <c r="R193" t="str">
         <f t="shared" si="5"/>
-        <v>L["Pet - Scalehide"] = "Familier - peau écailleuse"</v>
-      </c>
-    </row>
-    <row r="194" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Pet - Scalehide"] = "宠物 - 鳞甲类"</v>
+      </c>
+    </row>
+    <row r="194" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>2464</v>
       </c>
@@ -15254,10 +15253,10 @@
       </c>
       <c r="R194" t="str">
         <f t="shared" si="5"/>
-        <v>L["Shalassian"] = "shalassien"</v>
-      </c>
-    </row>
-    <row r="195" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Shalassian"] = "语言：夏拉斯语"</v>
+      </c>
+    </row>
+    <row r="195" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>2508</v>
       </c>
@@ -15297,10 +15296,10 @@
       </c>
       <c r="R195" t="str">
         <f t="shared" si="5"/>
-        <v>L["Legion Inscription"] = "Calligraphie de Legion"</v>
-      </c>
-    </row>
-    <row r="196" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Legion Inscription"] = "军团铭文"</v>
+      </c>
+    </row>
+    <row r="196" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>2526</v>
       </c>
@@ -15339,11 +15338,11 @@
         <v>{ entry = 2526, name = "Legion Leatherworking" },</v>
       </c>
       <c r="R196" t="str">
-        <f t="shared" ref="R196:R250" si="7">"L["""&amp;D196&amp;"""] = """ &amp; B196 &amp; """"</f>
-        <v>L["Legion Leatherworking"] = "Travail du cuir de Legion"</v>
-      </c>
-    </row>
-    <row r="197" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" ref="R196:R250" si="7">"L["""&amp;D196&amp;"""] = """ &amp; K196 &amp; """"</f>
+        <v>L["Legion Leatherworking"] = "军团制皮"</v>
+      </c>
+    </row>
+    <row r="197" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>2529</v>
       </c>
@@ -15383,10 +15382,10 @@
       </c>
       <c r="R197" t="str">
         <f t="shared" si="7"/>
-        <v>L["Cataclysm Leatherworking"] = "Travail du cuir de Cataclysm"</v>
-      </c>
-    </row>
-    <row r="198" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Cataclysm Leatherworking"] = "大地的裂变制皮"</v>
+      </c>
+    </row>
+    <row r="198" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>2530</v>
       </c>
@@ -15426,10 +15425,10 @@
       </c>
       <c r="R198" t="str">
         <f t="shared" si="7"/>
-        <v>L["Northrend Leatherworking"] = "Travail du cuir du Norfendre"</v>
-      </c>
-    </row>
-    <row r="199" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Northrend Leatherworking"] = "诺森德制皮"</v>
+      </c>
+    </row>
+    <row r="199" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>2531</v>
       </c>
@@ -15469,10 +15468,10 @@
       </c>
       <c r="R199" t="str">
         <f t="shared" si="7"/>
-        <v>L["Outland Leatherworking"] = "Travail du cuir d’Outreterre"</v>
-      </c>
-    </row>
-    <row r="200" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Outland Leatherworking"] = "外域制皮"</v>
+      </c>
+    </row>
+    <row r="200" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>2534</v>
       </c>
@@ -15512,10 +15511,10 @@
       </c>
       <c r="R200" t="str">
         <f t="shared" si="7"/>
-        <v>L["Legion Tailoring"] = "Couture de Legion"</v>
-      </c>
-    </row>
-    <row r="201" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Legion Tailoring"] = "军团裁缝"</v>
+      </c>
+    </row>
+    <row r="201" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>2535</v>
       </c>
@@ -15555,10 +15554,10 @@
       </c>
       <c r="R201" t="str">
         <f t="shared" si="7"/>
-        <v>L["Draenor Tailoring"] = "Couture de Draenor"</v>
-      </c>
-    </row>
-    <row r="202" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Draenor Tailoring"] = "德拉诺裁缝"</v>
+      </c>
+    </row>
+    <row r="202" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>2558</v>
       </c>
@@ -15598,10 +15597,10 @@
       </c>
       <c r="R202" t="str">
         <f t="shared" si="7"/>
-        <v>L["Legion Skinning"] = "Dépeçage de Legion"</v>
-      </c>
-    </row>
-    <row r="203" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Legion Skinning"] = "军团剥皮"</v>
+      </c>
+    </row>
+    <row r="203" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>2587</v>
       </c>
@@ -15641,7 +15640,7 @@
       </c>
       <c r="R203" t="str">
         <f t="shared" si="7"/>
-        <v>L["Draenor Fishing"] = "Pêche de Draenor"</v>
+        <v>L["Draenor Fishing"] = "德拉诺钓鱼"</v>
       </c>
     </row>
     <row r="204" spans="1:18" x14ac:dyDescent="0.25">
@@ -15684,7 +15683,7 @@
       </c>
       <c r="R204" t="str">
         <f t="shared" si="7"/>
-        <v>L["Pet - Toad"] = "Familier - crapaud"</v>
+        <v>L["Pet - Toad"] = "宠物 - 蟾蜍"</v>
       </c>
     </row>
     <row r="205" spans="1:18" x14ac:dyDescent="0.25">
@@ -15727,7 +15726,7 @@
       </c>
       <c r="R205" t="str">
         <f t="shared" si="7"/>
-        <v>L["Pet - Exotic Carapid"] = "Familier - carapide exotique"</v>
+        <v>L["Pet - Exotic Carapid"] = "宠物 - 步行虫（特殊）"</v>
       </c>
     </row>
     <row r="206" spans="1:18" x14ac:dyDescent="0.25">
@@ -15770,7 +15769,7 @@
       </c>
       <c r="R206" t="str">
         <f t="shared" si="7"/>
-        <v>L["Second Pet - Hunter"] = "Deuxième familier - chasseur"</v>
+        <v>L["Second Pet - Hunter"] = "第二宠物 - 猎人"</v>
       </c>
     </row>
     <row r="207" spans="1:18" x14ac:dyDescent="0.25">
@@ -15816,7 +15815,7 @@
         <v>L["Pet - Blood Beast"] = "Pet - Blood Beast"</v>
       </c>
     </row>
-    <row r="208" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>2751</v>
       </c>
@@ -15856,10 +15855,10 @@
       </c>
       <c r="R208" t="str">
         <f t="shared" si="7"/>
-        <v>L["Shadowlands Blacksmithing"] = "Forge d’Ombreterre"</v>
-      </c>
-    </row>
-    <row r="209" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Shadowlands Blacksmithing"] = "暗影界锻造"</v>
+      </c>
+    </row>
+    <row r="209" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>2753</v>
       </c>
@@ -15899,10 +15898,10 @@
       </c>
       <c r="R209" t="str">
         <f t="shared" si="7"/>
-        <v>L["Shadowlands Enchanting"] = "Enchantement d’Ombreterre"</v>
-      </c>
-    </row>
-    <row r="210" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Shadowlands Enchanting"] = "暗影界附魔"</v>
+      </c>
+    </row>
+    <row r="210" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>2759</v>
       </c>
@@ -15942,10 +15941,10 @@
       </c>
       <c r="R210" t="str">
         <f t="shared" si="7"/>
-        <v>L["Shadowlands Tailoring"] = "Couture d’Ombreterre"</v>
-      </c>
-    </row>
-    <row r="211" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Shadowlands Tailoring"] = "暗影界裁缝"</v>
+      </c>
+    </row>
+    <row r="211" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>2761</v>
       </c>
@@ -15985,10 +15984,10 @@
       </c>
       <c r="R211" t="str">
         <f t="shared" si="7"/>
-        <v>L["Shadowlands Mining"] = "Minage d’Ombreterre"</v>
-      </c>
-    </row>
-    <row r="212" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Shadowlands Mining"] = "暗影界采矿"</v>
+      </c>
+    </row>
+    <row r="212" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>2762</v>
       </c>
@@ -16028,7 +16027,7 @@
       </c>
       <c r="R212" t="str">
         <f t="shared" si="7"/>
-        <v>L["Shadowlands Skinning"] = "Dépeçage d’Ombreterre"</v>
+        <v>L["Shadowlands Skinning"] = "暗影界剥皮"</v>
       </c>
     </row>
     <row r="213" spans="1:18" x14ac:dyDescent="0.25">
@@ -16071,10 +16070,10 @@
       </c>
       <c r="R213" t="str">
         <f t="shared" si="7"/>
-        <v>L["Pet - Lesser Dragonkin"] = "Mascotte – Draconien inférieur"</v>
-      </c>
-    </row>
-    <row r="214" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Pet - Lesser Dragonkin"] = "宠物 - 次级龙类"</v>
+      </c>
+    </row>
+    <row r="214" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>905</v>
       </c>
@@ -16114,10 +16113,10 @@
       </c>
       <c r="R214" t="str">
         <f t="shared" si="7"/>
-        <v>L["Pandaren Neutral"] = "pandaren (neutre)"</v>
-      </c>
-    </row>
-    <row r="215" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Pandaren Neutral"] = "语言：熊猫人（中立）"</v>
+      </c>
+    </row>
+    <row r="215" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>2473</v>
       </c>
@@ -16157,10 +16156,10 @@
       </c>
       <c r="R215" t="str">
         <f t="shared" si="7"/>
-        <v>L["Pandaria Blacksmithing"] = "Forge de Pandarie"</v>
-      </c>
-    </row>
-    <row r="216" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Pandaria Blacksmithing"] = "潘达利亚锻造"</v>
+      </c>
+    </row>
+    <row r="216" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>2511</v>
       </c>
@@ -16200,10 +16199,10 @@
       </c>
       <c r="R216" t="str">
         <f t="shared" si="7"/>
-        <v>L["Cataclysm Inscription"] = "Calligraphie de Cataclysm"</v>
-      </c>
-    </row>
-    <row r="217" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Cataclysm Inscription"] = "大地的裂变铭文"</v>
+      </c>
+    </row>
+    <row r="217" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>2512</v>
       </c>
@@ -16243,10 +16242,10 @@
       </c>
       <c r="R217" t="str">
         <f t="shared" si="7"/>
-        <v>L["Northrend Inscription"] = "Calligraphie du Norfendre"</v>
-      </c>
-    </row>
-    <row r="218" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Northrend Inscription"] = "诺森德铭文"</v>
+      </c>
+    </row>
+    <row r="218" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>2517</v>
       </c>
@@ -16286,10 +16285,10 @@
       </c>
       <c r="R218" t="str">
         <f t="shared" si="7"/>
-        <v>L["Kul Tiran Jewelcrafting"] = "Joaillerie de Kul Tiras"</v>
-      </c>
-    </row>
-    <row r="219" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Kul Tiran Jewelcrafting"] = "库尔提拉斯珠宝加工"</v>
+      </c>
+    </row>
+    <row r="219" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>2519</v>
       </c>
@@ -16329,10 +16328,10 @@
       </c>
       <c r="R219" t="str">
         <f t="shared" si="7"/>
-        <v>L["Draenor Jewelcrafting"] = "Joaillerie de Draenor"</v>
-      </c>
-    </row>
-    <row r="220" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Draenor Jewelcrafting"] = "德拉诺珠宝加工"</v>
+      </c>
+    </row>
+    <row r="220" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>2550</v>
       </c>
@@ -16372,10 +16371,10 @@
       </c>
       <c r="R220" t="str">
         <f t="shared" si="7"/>
-        <v>L["Legion Herbalism"] = "Herboristerie de Legion"</v>
-      </c>
-    </row>
-    <row r="221" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Legion Herbalism"] = "军团草药学"</v>
+      </c>
+    </row>
+    <row r="221" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>2559</v>
       </c>
@@ -16415,7 +16414,7 @@
       </c>
       <c r="R221" t="str">
         <f t="shared" si="7"/>
-        <v>L["Draenor Skinning"] = "Dépeçage de Draenor"</v>
+        <v>L["Draenor Skinning"] = "德拉诺剥皮"</v>
       </c>
     </row>
     <row r="222" spans="1:18" x14ac:dyDescent="0.25">
@@ -16458,10 +16457,10 @@
       </c>
       <c r="R222" t="str">
         <f t="shared" si="7"/>
-        <v>L["Pet - Lizard"] = "Familier - lézard"</v>
-      </c>
-    </row>
-    <row r="223" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Pet - Lizard"] = "宠物 - 蜥蜴"</v>
+      </c>
+    </row>
+    <row r="223" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>2817</v>
       </c>
@@ -16501,10 +16500,10 @@
       </c>
       <c r="R223" t="str">
         <f t="shared" si="7"/>
-        <v>L["Cypher"] = "cryptogramme"</v>
-      </c>
-    </row>
-    <row r="224" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Cypher"] = "语言：密文"</v>
+      </c>
+    </row>
+    <row r="224" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>2826</v>
       </c>
@@ -16544,10 +16543,10 @@
       </c>
       <c r="R224" t="str">
         <f t="shared" si="7"/>
-        <v>L["Dragon Isles Fishing"] = "Pêche des îles aux Dragons"</v>
-      </c>
-    </row>
-    <row r="225" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Dragon Isles Fishing"] = "巨龙群岛钓鱼"</v>
+      </c>
+    </row>
+    <row r="225" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>2870</v>
       </c>
@@ -16587,10 +16586,10 @@
       </c>
       <c r="R225" t="str">
         <f t="shared" si="7"/>
-        <v>L["Shipment Prototype"] = "Prototype de cargaison"</v>
-      </c>
-    </row>
-    <row r="226" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Shipment Prototype"] = "货物原型"</v>
+      </c>
+    </row>
+    <row r="226" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>673</v>
       </c>
@@ -16630,10 +16629,10 @@
       </c>
       <c r="R226" t="str">
         <f t="shared" si="7"/>
-        <v>L["Forsaken"] = "réprouvé"</v>
-      </c>
-    </row>
-    <row r="227" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Forsaken"] = "语言：亡灵语"</v>
+      </c>
+    </row>
+    <row r="227" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>759</v>
       </c>
@@ -16673,10 +16672,10 @@
       </c>
       <c r="R227" t="str">
         <f t="shared" si="7"/>
-        <v>L["Draenei"] = "draeneï"</v>
-      </c>
-    </row>
-    <row r="228" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Draenei"] = "语言：德莱尼语"</v>
+      </c>
+    </row>
+    <row r="228" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>792</v>
       </c>
@@ -16716,7 +16715,7 @@
       </c>
       <c r="R228" t="str">
         <f t="shared" si="7"/>
-        <v>L["Goblin"] = "gobelin"</v>
+        <v>L["Goblin"] = "语言：地精语"</v>
       </c>
     </row>
     <row r="229" spans="1:18" x14ac:dyDescent="0.25">
@@ -16759,7 +16758,7 @@
       </c>
       <c r="R229" t="str">
         <f t="shared" si="7"/>
-        <v>L["Pet - Water Elemental Minor Talent Version"] = "Pet - Water Elemental Minor Talent Version"</v>
+        <v>L["Pet - Water Elemental Minor Talent Version"] = "宠物 - 水元素（次级天赋版）"</v>
       </c>
     </row>
     <row r="230" spans="1:18" x14ac:dyDescent="0.25">
@@ -16802,10 +16801,10 @@
       </c>
       <c r="R230" t="str">
         <f t="shared" si="7"/>
-        <v>L["Pet - Feathermane"] = "Familier - Crin-de-plume"</v>
-      </c>
-    </row>
-    <row r="231" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Pet - Feathermane"] = "宠物 - 羽鬃兽"</v>
+      </c>
+    </row>
+    <row r="231" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>2465</v>
       </c>
@@ -16845,10 +16844,10 @@
       </c>
       <c r="R231" t="str">
         <f t="shared" si="7"/>
-        <v>L["Thalassian"] = "thalassien"</v>
-      </c>
-    </row>
-    <row r="232" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Thalassian"] = "语言：萨拉斯语"</v>
+      </c>
+    </row>
+    <row r="232" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>2474</v>
       </c>
@@ -16888,10 +16887,10 @@
       </c>
       <c r="R232" t="str">
         <f t="shared" si="7"/>
-        <v>L["Cataclysm Blacksmithing"] = "Forge de Cataclysm"</v>
-      </c>
-    </row>
-    <row r="233" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Cataclysm Blacksmithing"] = "大地的裂变锻造"</v>
+      </c>
+    </row>
+    <row r="233" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>2483</v>
       </c>
@@ -16931,10 +16930,10 @@
       </c>
       <c r="R233" t="str">
         <f t="shared" si="7"/>
-        <v>L["Northrend Alchemy"] = "Alchimie du Norfendre"</v>
-      </c>
-    </row>
-    <row r="234" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Northrend Alchemy"] = "诺森德炼金"</v>
+      </c>
+    </row>
+    <row r="234" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>2489</v>
       </c>
@@ -16974,10 +16973,10 @@
       </c>
       <c r="R234" t="str">
         <f t="shared" si="7"/>
-        <v>L["Pandaria Enchanting"] = "Enchantement de Pandarie"</v>
-      </c>
-    </row>
-    <row r="235" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Pandaria Enchanting"] = "潘达利亚附魔"</v>
+      </c>
+    </row>
+    <row r="235" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>2509</v>
       </c>
@@ -17017,10 +17016,10 @@
       </c>
       <c r="R235" t="str">
         <f t="shared" si="7"/>
-        <v>L["Draenor Inscription"] = "Calligraphie de Draenor"</v>
-      </c>
-    </row>
-    <row r="236" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Draenor Inscription"] = "德拉诺铭文"</v>
+      </c>
+    </row>
+    <row r="236" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>2514</v>
       </c>
@@ -17060,10 +17059,10 @@
       </c>
       <c r="R236" t="str">
         <f t="shared" si="7"/>
-        <v>L["Classic Inscription"] = "Calligraphie classique"</v>
-      </c>
-    </row>
-    <row r="237" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Classic Inscription"] = "经典旧世铭文"</v>
+      </c>
+    </row>
+    <row r="237" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>2541</v>
       </c>
@@ -17103,10 +17102,10 @@
       </c>
       <c r="R237" t="str">
         <f t="shared" si="7"/>
-        <v>L["Kul Tiran Cooking"] = "Cuisine de Kul Tiras"</v>
-      </c>
-    </row>
-    <row r="238" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Kul Tiran Cooking"] = "库尔提拉斯烹饪"</v>
+      </c>
+    </row>
+    <row r="238" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>2589</v>
       </c>
@@ -17146,10 +17145,10 @@
       </c>
       <c r="R238" t="str">
         <f t="shared" si="7"/>
-        <v>L["Cataclysm Fishing"] = "Pêche de Cataclysm"</v>
-      </c>
-    </row>
-    <row r="239" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Cataclysm Fishing"] = "大地的裂变钓鱼"</v>
+      </c>
+    </row>
+    <row r="239" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>2750</v>
       </c>
@@ -17189,10 +17188,10 @@
       </c>
       <c r="R239" t="str">
         <f t="shared" si="7"/>
-        <v>L["Shadowlands Alchemy"] = "Alchimie d’Ombreterre"</v>
-      </c>
-    </row>
-    <row r="240" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Shadowlands Alchemy"] = "暗影界炼金术"</v>
+      </c>
+    </row>
+    <row r="240" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>2777</v>
       </c>
@@ -17232,7 +17231,7 @@
       </c>
       <c r="R240" t="str">
         <f t="shared" si="7"/>
-        <v>L["Soul Cyphering"] = "Cryptogrammes d’âmes"</v>
+        <v>L["Soul Cyphering"] = "灵魂密文"</v>
       </c>
     </row>
     <row r="241" spans="1:18" x14ac:dyDescent="0.25">
@@ -17275,7 +17274,7 @@
       </c>
       <c r="R241" t="str">
         <f t="shared" si="7"/>
-        <v>L["Pet - Courser"] = "Familier - coursier"</v>
+        <v>L["Pet - Courser"] = "宠物 - 骏马"</v>
       </c>
     </row>
     <row r="242" spans="1:18" x14ac:dyDescent="0.25">
@@ -17318,10 +17317,10 @@
       </c>
       <c r="R242" t="str">
         <f t="shared" si="7"/>
-        <v>L["Pet - Camel"] = "Familier - dromadaire"</v>
-      </c>
-    </row>
-    <row r="243" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Pet - Camel"] = "宠物 - 骆驼"</v>
+      </c>
+    </row>
+    <row r="243" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>2827</v>
       </c>
@@ -17361,10 +17360,10 @@
       </c>
       <c r="R243" t="str">
         <f t="shared" si="7"/>
-        <v>L["Dragon Isles Engineering"] = "Ingénierie des îles aux Dragons"</v>
-      </c>
-    </row>
-    <row r="244" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Dragon Isles Engineering"] = "巨龙群岛工程学"</v>
+      </c>
+    </row>
+    <row r="244" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>2886</v>
       </c>
@@ -17404,10 +17403,10 @@
       </c>
       <c r="R244" t="str">
         <f t="shared" si="7"/>
-        <v>L["Supply Shipments"] = "Cargaisons de ravitaillement"</v>
-      </c>
-    </row>
-    <row r="245" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Supply Shipments"] = "补给货物"</v>
+      </c>
+    </row>
+    <row r="245" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>115</v>
       </c>
@@ -17447,10 +17446,10 @@
       </c>
       <c r="R245" t="str">
         <f t="shared" si="7"/>
-        <v>L["Taurahe"] = "taurahe"</v>
-      </c>
-    </row>
-    <row r="246" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Taurahe"] = "语言：牛头人语"</v>
+      </c>
+    </row>
+    <row r="246" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>934</v>
       </c>
@@ -17490,10 +17489,10 @@
       </c>
       <c r="R246" t="str">
         <f t="shared" si="7"/>
-        <v>L["All - Specializations"] = "Tous - Spécialisations"</v>
-      </c>
-    </row>
-    <row r="247" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["All - Specializations"] = "全部专精"</v>
+      </c>
+    </row>
+    <row r="247" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>2487</v>
       </c>
@@ -17533,10 +17532,10 @@
       </c>
       <c r="R247" t="str">
         <f t="shared" si="7"/>
-        <v>L["Legion Enchanting"] = "Enchantement de Legion"</v>
-      </c>
-    </row>
-    <row r="248" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Legion Enchanting"] = "军团附魔"</v>
+      </c>
+    </row>
+    <row r="248" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>2492</v>
       </c>
@@ -17576,10 +17575,10 @@
       </c>
       <c r="R248" t="str">
         <f t="shared" si="7"/>
-        <v>L["Northrend Enchanting"] = "Enchantement du Norfendre"</v>
-      </c>
-    </row>
-    <row r="249" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Northrend Enchanting"] = "诺森德附魔"</v>
+      </c>
+    </row>
+    <row r="249" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>2518</v>
       </c>
@@ -17619,10 +17618,10 @@
       </c>
       <c r="R249" t="str">
         <f t="shared" si="7"/>
-        <v>L["Legion Jewelcrafting"] = "Joaillerie de Legion"</v>
-      </c>
-    </row>
-    <row r="250" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>L["Legion Jewelcrafting"] = "军团珠宝加工"</v>
+      </c>
+    </row>
+    <row r="250" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>2811</v>
       </c>
@@ -17662,17 +17661,11 @@
       </c>
       <c r="R250" t="str">
         <f t="shared" si="7"/>
-        <v>L["Stygia Crafting"] = "Travail des stygies"</v>
+        <v>L["Stygia Crafting"] = "冥殇制作"</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:K250" xr:uid="{03F8331B-0190-47B4-AA03-F9BBE88A2224}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Techniques de familier"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A2:K250" xr:uid="{03F8331B-0190-47B4-AA03-F9BBE88A2224}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>